<commit_message>
Added Report Title option and dropdown in sheet also
</commit_message>
<xml_diff>
--- a/services/api/templates/report_template.xlsx
+++ b/services/api/templates/report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniketsandhan/Desktop/PDF_Marker/services/api/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E78F4AFB-3342-604E-9A76-BE7F52911338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1365FE9-727D-E74A-B6FC-39310DFE5157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ID:</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Title: </t>
   </si>
 </sst>
 </file>
@@ -112,30 +115,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Roboto Serif"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +169,14 @@
         <bgColor rgb="FF9FC5E8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -252,11 +261,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -264,13 +299,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -299,6 +337,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -707,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB14984E-B5B3-2140-A9B9-7EC704D00214}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -740,162 +781,174 @@
     </row>
     <row r="3" spans="1:7" ht="17" thickBot="1">
       <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="17" thickBot="1">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="17" thickBot="1">
-      <c r="A5" s="10" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="17" thickBot="1">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1">
-      <c r="A6" s="15" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="17" thickBot="1">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" thickBot="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1">
+    <row r="8" spans="1:7" ht="18" thickBot="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="C8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7" ht="17" thickBot="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" ht="17" thickBot="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" ht="17" thickBot="1">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7" ht="17" thickBot="1">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+  <mergeCells count="14">
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="E6:G6"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Drawing Number level modification both in viewer and editor end
</commit_message>
<xml_diff>
--- a/services/api/templates/report_template.xlsx
+++ b/services/api/templates/report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniketsandhan/Desktop/PDF_Marker/services/api/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9908BB3C-0EEF-BA47-9691-9274D507CB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7030B04-95FC-2841-8946-88DA23D44A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
+    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ID:</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Instrument</t>
+  </si>
+  <si>
+    <t>Inspection Point</t>
   </si>
 </sst>
 </file>
@@ -294,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -302,9 +305,27 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -323,32 +344,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,40 +754,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB14984E-B5B3-2140-A9B9-7EC704D00214}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickBot="1">
-      <c r="A1" s="5" t="e" vm="1">
+    <row r="1" spans="1:9" ht="17" thickBot="1">
+      <c r="A1" s="11" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" ht="17" thickBot="1">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1">
       <c r="A3" s="17" t="s">
         <v>13</v>
       </c>
@@ -792,86 +801,94 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" ht="17" thickBot="1">
-      <c r="A4" s="8" t="s">
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="16" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" customHeight="1">
+      <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" ht="17" customHeight="1" thickBot="1">
-      <c r="A6" s="13" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" ht="17" customHeight="1" thickBot="1">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" ht="17" thickBot="1">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="17" thickBot="1">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" thickBot="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="1:9" ht="18" thickBot="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="17" thickBot="1">
+      <c r="F8" s="10"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="17" thickBot="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -880,8 +897,9 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="17" thickBot="1">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -890,8 +908,9 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="17" thickBot="1">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="17" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -900,8 +919,9 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="17" thickBot="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -910,8 +930,9 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="17" thickBot="1">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="17" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -920,8 +941,9 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="17" thickBot="1">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="17" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -930,8 +952,9 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="17" thickBot="1">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="17" thickBot="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -940,8 +963,9 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="17" thickBot="1">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="17" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -950,23 +974,25 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="E6:H6"/>
+  <mergeCells count="15">
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E6:I6"/>
     <mergeCell ref="G7:G8"/>
+    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
OCR values will be saved now, included in reports, also made status drop down with conditional formating
</commit_message>
<xml_diff>
--- a/services/api/templates/report_template.xlsx
+++ b/services/api/templates/report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniketsandhan/Desktop/PDF_Marker/services/api/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB19956-23D2-FB45-8CA8-0441D097E0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94C2E1-5FD1-D94A-9435-86BA968D247B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
+    <workbookView xWindow="13100" yWindow="1140" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Created By:</t>
   </si>
   <si>
-    <t>MarkSet Name:</t>
-  </si>
-  <si>
     <t>Created At:</t>
   </si>
   <si>
@@ -105,14 +102,17 @@
     <t>Instrument</t>
   </si>
   <si>
-    <t>Inspection Point</t>
+    <t>Inspection Map Name:</t>
+  </si>
+  <si>
+    <t>Inspection Reference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,15 +133,29 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Roboto Serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Roboto Serif"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -182,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -293,16 +307,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -314,48 +352,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,7 +796,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -790,103 +829,103 @@
       <c r="H2" s="5"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="17" thickBot="1">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:9" ht="23" thickBot="1">
+      <c r="A3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1">
+      <c r="A4" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="17" customHeight="1" thickBot="1">
+      <c r="A6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" ht="17" thickBot="1">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" ht="17" thickBot="1">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="16" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" thickBot="1">
-      <c r="A6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" ht="17" thickBot="1">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="I7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="9" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="18" thickBot="1">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="18" thickBot="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="17" thickBot="1">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
Solved Map downloading and removed OCR filtering
</commit_message>
<xml_diff>
--- a/services/api/templates/report_template.xlsx
+++ b/services/api/templates/report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniketsandhan/Desktop/PDF_Marker/services/api/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94C2E1-5FD1-D94A-9435-86BA968D247B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640F2291-6F53-DD45-80FC-85A3B803B23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="1140" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
+    <workbookView xWindow="11320" yWindow="1040" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,26 +173,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FFE0BC6A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6FA8DC"/>
+        <fgColor rgb="FF82CCEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF82CCEC"/>
         <bgColor rgb="FF6FA8DC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9FC5E8"/>
+        <fgColor rgb="FF82CCEC"/>
         <bgColor rgb="FF9FC5E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -340,67 +340,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF82CCEC"/>
+      <color rgb="FFE0BC6A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -796,7 +802,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -806,126 +812,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" thickBot="1">
-      <c r="A1" s="3" t="e" vm="1">
+      <c r="A1" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="17" thickBot="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="23" thickBot="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="17" thickBot="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="16" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" ht="17" customHeight="1" thickBot="1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="15" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" ht="17" thickBot="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="19"/>
+      <c r="F7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" thickBot="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="2" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" ht="17" thickBot="1">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
Circle size reduced and Eye icon and hash icon added
</commit_message>
<xml_diff>
--- a/services/api/templates/report_template.xlsx
+++ b/services/api/templates/report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniketsandhan/Desktop/PDF_Marker/services/api/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640F2291-6F53-DD45-80FC-85A3B803B23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50FE43C-52CA-B444-B410-3F70024CF04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="1040" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
+    <workbookView xWindow="1160" yWindow="1040" windowWidth="27640" windowHeight="15840" xr2:uid="{5650C91F-4D76-E04A-93D0-95AE0999C9B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID:</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>Inspection Reference</t>
+  </si>
+  <si>
+    <t>To view complete PDF click:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +160,11 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos SemiBold"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -196,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -331,15 +339,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -354,30 +387,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,14 +395,35 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB14984E-B5B3-2140-A9B9-7EC704D00214}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -811,129 +841,137 @@
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1">
-      <c r="A1" s="2" t="e" vm="1">
+    <row r="1" spans="1:16" ht="17" thickBot="1">
+      <c r="A1" s="6" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="23" thickBot="1">
-      <c r="A3" s="16" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="5"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" ht="23" thickBot="1">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-    </row>
-    <row r="4" spans="1:9" ht="17" thickBot="1">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:16" ht="17" thickBot="1">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="16" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" ht="16" customHeight="1">
+      <c r="A5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" thickBot="1">
-      <c r="A6" s="12" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:16" ht="17" customHeight="1" thickBot="1">
+      <c r="A6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" ht="17" thickBot="1">
-      <c r="A7" s="19" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:16" ht="17" thickBot="1">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18" thickBot="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="22" t="s">
+    <row r="8" spans="1:16" ht="18" thickBot="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" ht="17" thickBot="1">
+      <c r="F8" s="16"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:16" ht="17" thickBot="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -944,7 +982,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1">
+    <row r="10" spans="1:16" ht="17" thickBot="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -955,7 +993,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="17" thickBot="1">
+    <row r="11" spans="1:16" ht="17" thickBot="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -966,7 +1004,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="17" thickBot="1">
+    <row r="12" spans="1:16" ht="17" thickBot="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -977,7 +1015,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="17" thickBot="1">
+    <row r="13" spans="1:16" ht="17" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -988,7 +1026,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1">
+    <row r="14" spans="1:16" ht="17" thickBot="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -999,7 +1037,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1">
+    <row r="15" spans="1:16" ht="17" thickBot="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1010,7 +1048,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1">
+    <row r="16" spans="1:16" ht="17" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1022,7 +1060,11 @@
       <c r="I16" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="K1:P1"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A3:I3"/>
@@ -1035,9 +1077,6 @@
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E5:I5"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>